<commit_message>
Analysis done for no solution
</commit_message>
<xml_diff>
--- a/Analysis.xlsx
+++ b/Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashwi\Desktop\DSA Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD9CDC3E-2161-430E-A57C-B16B28482666}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6217D6CB-2DEA-4C8E-AC33-3D8AEC73B613}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -362,10 +362,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D51"/>
+  <dimension ref="A1:D70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="E66" sqref="E66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -675,19 +675,134 @@
         <v>109</v>
       </c>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B49">
         <v>116</v>
       </c>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B50">
         <v>110</v>
       </c>
     </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B51">
         <v>90</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>15</v>
+      </c>
+      <c r="B52">
+        <v>107</v>
+      </c>
+      <c r="C52">
+        <f>AVERAGE(B52:B60)</f>
+        <v>120.55555555555556</v>
+      </c>
+      <c r="D52">
+        <v>0.1206</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B53">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B54">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B55">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B56">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B57">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B58">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B59">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B60">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>20</v>
+      </c>
+      <c r="B61">
+        <v>108</v>
+      </c>
+      <c r="C61">
+        <f>AVERAGE(B61:B70)</f>
+        <v>113.6</v>
+      </c>
+      <c r="D61">
+        <v>0.11360000000000001</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B62">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B63">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B64">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B65">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B66">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B67">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="68" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B68">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="69" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B69">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="70" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B70">
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>